<commit_message>
DELPHI-247 Log changes to comments of our users
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/documents/ActivityLogEvents.xlsx
+++ b/src/main/webapp/resources/documents/ActivityLogEvents.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hle\Documents\EUSurvey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lust\IdeaProjects\eusurvey-delphi\src\main\webapp\resources\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B084E5C3-45A6-4AE3-9F3B-06F89421B188}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>102 - Survey - Survey successfully imported</t>
   </si>
@@ -269,20 +270,23 @@
     <t>701 - Messages - End notification message sent</t>
   </si>
   <si>
-    <t>Save</t>
-  </si>
-  <si>
     <t>101 - Survey - Survey successfully created</t>
   </si>
   <si>
     <t>Activity Log events</t>
+  </si>
+  <si>
+    <t>801 - Comments - Comment modified</t>
+  </si>
+  <si>
+    <t>802 - Comments - Comment deleted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,21 +304,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF333333"/>
+      <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF666666"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -388,19 +387,13 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -412,6 +405,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -419,6 +418,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF666666"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -692,29 +696,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B87"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:B99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.85546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
-        <v>83</v>
+      <c r="B2" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="7"/>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" spans="2:2" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
-        <v>82</v>
+      <c r="B4" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="28.5" x14ac:dyDescent="0.25">
@@ -1122,13 +1126,51 @@
         <v>80</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="3"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="4" t="s">
-        <v>81</v>
-      </c>
+    <row r="86" spans="2:2" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B86" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B87" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="8"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" s="8"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" s="8"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" s="8"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" s="8"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" s="8"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" s="8"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" s="8"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96" s="8"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" s="8"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" s="8"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>